<commit_message>
Abundance Search Feature Completed
</commit_message>
<xml_diff>
--- a/Docs/Datasets/Abundance.xlsx
+++ b/Docs/Datasets/Abundance.xlsx
@@ -686,9 +686,6 @@
     <t>Sharks (various species)</t>
   </si>
   <si>
-    <t>Kerela</t>
-  </si>
-  <si>
     <t>Gujarat</t>
   </si>
   <si>
@@ -981,6 +978,9 @@
   </si>
   <si>
     <t>little tunny</t>
+  </si>
+  <si>
+    <t>Kerala</t>
   </si>
 </sst>
 </file>
@@ -27242,8 +27242,8 @@
   </sheetPr>
   <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="D245" sqref="D245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -27253,1288 +27253,1288 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>289</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="29" t="s">
-        <v>223</v>
+        <v>321</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75">
       <c r="A31" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75">
       <c r="A32" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75">
       <c r="A33" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75">
       <c r="A34" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75">
       <c r="A35" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12.75">
       <c r="A36" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75">
       <c r="A37" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75">
       <c r="A38" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75">
       <c r="A39" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="12.75">
       <c r="A40" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="12.75">
       <c r="A41" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="12.75">
       <c r="A42" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75">
       <c r="A43" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12.75">
       <c r="A44" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75">
       <c r="A45" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75">
       <c r="A46" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="12.75">
       <c r="A47" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75">
       <c r="A48" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="12.75">
       <c r="A49" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="12.75">
       <c r="A50" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="12.75">
       <c r="A51" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="12.75">
       <c r="A52" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="12.75">
       <c r="A53" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="12.75">
       <c r="A54" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="12.75">
       <c r="A55" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="12.75">
       <c r="A56" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.75">
       <c r="A57" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15">
       <c r="A58" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15">
       <c r="A59" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15">
       <c r="A60" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C60" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15">
       <c r="A61" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15">
       <c r="A62" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15">
       <c r="A63" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15">
       <c r="A64" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15">
       <c r="A65" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.75">
       <c r="A66" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="12.75">
       <c r="A67" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="12.75">
       <c r="A68" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="12.75">
       <c r="A69" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="12.75">
       <c r="A70" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="12.75">
       <c r="A71" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="12.75">
       <c r="A72" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="12.75">
       <c r="A73" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.75">
       <c r="A74" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="12.75">
       <c r="A75" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="12.75">
       <c r="A76" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="12.75">
       <c r="A77" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="12.75">
       <c r="A78" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.75">
       <c r="A79" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="12.75">
       <c r="A80" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="12.75">
       <c r="A81" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="12.75">
       <c r="A82" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="12.75">
       <c r="A83" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="12.75">
       <c r="A84" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E84" s="11"/>
     </row>
     <row r="85" spans="1:5" ht="12.75">
       <c r="A85" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C85" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E85" s="11"/>
     </row>
     <row r="86" spans="1:5" ht="12.75">
       <c r="A86" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E86" s="11"/>
     </row>
     <row r="87" spans="1:5" ht="12.75">
       <c r="A87" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E87" s="11"/>
     </row>
     <row r="88" spans="1:5" ht="12.75">
       <c r="A88" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E88" s="11"/>
     </row>
     <row r="89" spans="1:5" ht="12.75">
       <c r="A89" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:5" ht="12.75">
       <c r="A90" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E90" s="11"/>
     </row>
     <row r="91" spans="1:5" ht="12.75">
       <c r="A91" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E91" s="11"/>
     </row>
     <row r="92" spans="1:5" ht="12.75">
       <c r="A92" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" ht="12.75">
       <c r="A93" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C93" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E93" s="11"/>
     </row>
     <row r="94" spans="1:5" ht="12.75">
       <c r="A94" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B94" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C94" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="14.25">
       <c r="A95" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B95" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B95" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C95" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15">
       <c r="A96" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B96" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B96" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C96" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15">
       <c r="A97" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B97" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B97" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C97" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25">
       <c r="A98" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B98" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B98" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C98" s="28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75">
       <c r="A99" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B99" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B99" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C99" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75">
       <c r="A100" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B100" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B100" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C100" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75">
       <c r="A101" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B101" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B101" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C101" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75">
       <c r="A102" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B102" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B102" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C102" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75">
       <c r="A103" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B103" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B103" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C103" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75">
       <c r="A104" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B104" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B104" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C104" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75">
       <c r="A105" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B105" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="B105" s="23" t="s">
-        <v>226</v>
-      </c>
       <c r="C105" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75">
       <c r="A106" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75">
       <c r="A107" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75">
       <c r="A108" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75">
       <c r="A109" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75">
       <c r="A110" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15">
       <c r="A111" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C111" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15">
       <c r="A112" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B112" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C112" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75">
       <c r="A113" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75">
       <c r="A114" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B114" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C114" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75">
       <c r="A115" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B115" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C115" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="12.75">
       <c r="A116" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B116" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="15">
@@ -28542,10 +28542,10 @@
         <v>93</v>
       </c>
       <c r="B117" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C117" s="25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15">
@@ -28553,10 +28553,10 @@
         <v>93</v>
       </c>
       <c r="B118" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C118" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75">
@@ -28564,10 +28564,10 @@
         <v>93</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15">
@@ -28575,10 +28575,10 @@
         <v>93</v>
       </c>
       <c r="B120" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C120" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15">
@@ -28586,10 +28586,10 @@
         <v>93</v>
       </c>
       <c r="B121" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C121" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75">
@@ -28597,10 +28597,10 @@
         <v>93</v>
       </c>
       <c r="B122" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75">
@@ -28608,10 +28608,10 @@
         <v>93</v>
       </c>
       <c r="B123" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C123" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="12.75">
@@ -28619,10 +28619,10 @@
         <v>93</v>
       </c>
       <c r="B124" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C124" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75">
@@ -28630,10 +28630,10 @@
         <v>93</v>
       </c>
       <c r="B125" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C125" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75">
@@ -28641,10 +28641,10 @@
         <v>93</v>
       </c>
       <c r="B126" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C126" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75">
@@ -28652,10 +28652,10 @@
         <v>93</v>
       </c>
       <c r="B127" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15">
@@ -28663,10 +28663,10 @@
         <v>93</v>
       </c>
       <c r="B128" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C128" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="15">
@@ -28674,10 +28674,10 @@
         <v>93</v>
       </c>
       <c r="B129" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C129" s="25" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15">
@@ -28685,10 +28685,10 @@
         <v>93</v>
       </c>
       <c r="B130" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C130" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="15">
@@ -28696,10 +28696,10 @@
         <v>93</v>
       </c>
       <c r="B131" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C131" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15">
@@ -28707,10 +28707,10 @@
         <v>93</v>
       </c>
       <c r="B132" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C132" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="12.75">
@@ -28718,10 +28718,10 @@
         <v>93</v>
       </c>
       <c r="B133" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="12.75">
@@ -28729,10 +28729,10 @@
         <v>93</v>
       </c>
       <c r="B134" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15">
@@ -28740,10 +28740,10 @@
         <v>93</v>
       </c>
       <c r="B135" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C135" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15">
@@ -28751,10 +28751,10 @@
         <v>93</v>
       </c>
       <c r="B136" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C136" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15">
@@ -28762,10 +28762,10 @@
         <v>93</v>
       </c>
       <c r="B137" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C137" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15">
@@ -28773,10 +28773,10 @@
         <v>93</v>
       </c>
       <c r="B138" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C138" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="12.75">
@@ -28784,109 +28784,109 @@
         <v>93</v>
       </c>
       <c r="B139" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C139" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="12.75">
       <c r="A140" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="12.75">
       <c r="A141" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B141" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C141" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="12.75">
       <c r="A142" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C142" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="12.75">
       <c r="A143" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C143" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="12.75">
       <c r="A144" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C144" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="12.75">
       <c r="A145" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C145" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="12.75">
       <c r="A146" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C146" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="12.75">
       <c r="A147" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C147" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="12.75">
       <c r="A148" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C148" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="12.75">
@@ -28894,10 +28894,10 @@
         <v>115</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C149" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="12.75">
@@ -28905,10 +28905,10 @@
         <v>115</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C150" s="23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="12.75">
@@ -28916,10 +28916,10 @@
         <v>115</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C151" s="23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="12.75">
@@ -28927,10 +28927,10 @@
         <v>115</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C152" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="12.75">
@@ -28938,10 +28938,10 @@
         <v>115</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C153" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="12.75">
@@ -28949,10 +28949,10 @@
         <v>115</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C154" s="23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="12.75">
@@ -28960,10 +28960,10 @@
         <v>115</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C155" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="12.75">
@@ -28971,10 +28971,10 @@
         <v>115</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C156" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="12.75">
@@ -28982,10 +28982,10 @@
         <v>115</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C157" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="12.75">
@@ -28993,10 +28993,10 @@
         <v>115</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C158" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="12.75">
@@ -29004,10 +29004,10 @@
         <v>115</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C159" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="12.75">
@@ -29015,10 +29015,10 @@
         <v>115</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C160" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="12.75">
@@ -29026,10 +29026,10 @@
         <v>115</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C161" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="12.75">
@@ -29037,10 +29037,10 @@
         <v>115</v>
       </c>
       <c r="B162" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C162" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="12.75">
@@ -29048,10 +29048,10 @@
         <v>115</v>
       </c>
       <c r="B163" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C163" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="12.75">
@@ -29059,10 +29059,10 @@
         <v>115</v>
       </c>
       <c r="B164" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C164" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="12.75">
@@ -29070,10 +29070,10 @@
         <v>115</v>
       </c>
       <c r="B165" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C165" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="12.75">
@@ -29081,10 +29081,10 @@
         <v>115</v>
       </c>
       <c r="B166" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C166" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="12.75">
@@ -29092,10 +29092,10 @@
         <v>115</v>
       </c>
       <c r="B167" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C167" s="23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="12.75">
@@ -29103,10 +29103,10 @@
         <v>115</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C168" s="23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="12.75">
@@ -29114,10 +29114,10 @@
         <v>115</v>
       </c>
       <c r="B169" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C169" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="12.75">
@@ -29125,10 +29125,10 @@
         <v>115</v>
       </c>
       <c r="B170" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C170" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="12.75">
@@ -29136,10 +29136,10 @@
         <v>127</v>
       </c>
       <c r="B171" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C171" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="12.75">
@@ -29147,10 +29147,10 @@
         <v>127</v>
       </c>
       <c r="B172" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C172" s="23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="12.75">
@@ -29158,10 +29158,10 @@
         <v>127</v>
       </c>
       <c r="B173" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C173" s="23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="12.75">
@@ -29169,10 +29169,10 @@
         <v>127</v>
       </c>
       <c r="B174" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C174" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="12.75">
@@ -29180,10 +29180,10 @@
         <v>127</v>
       </c>
       <c r="B175" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C175" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="12.75">
@@ -29191,10 +29191,10 @@
         <v>127</v>
       </c>
       <c r="B176" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C176" s="23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="12.75">
@@ -29202,10 +29202,10 @@
         <v>127</v>
       </c>
       <c r="B177" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C177" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="12.75">
@@ -29213,10 +29213,10 @@
         <v>127</v>
       </c>
       <c r="B178" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C178" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="12.75">
@@ -29224,10 +29224,10 @@
         <v>127</v>
       </c>
       <c r="B179" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C179" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="12.75">
@@ -29235,10 +29235,10 @@
         <v>127</v>
       </c>
       <c r="B180" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C180" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="12.75">
@@ -29246,10 +29246,10 @@
         <v>127</v>
       </c>
       <c r="B181" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C181" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="12.75">
@@ -29257,10 +29257,10 @@
         <v>127</v>
       </c>
       <c r="B182" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C182" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="12.75">
@@ -29268,10 +29268,10 @@
         <v>127</v>
       </c>
       <c r="B183" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C183" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="12.75">
@@ -29279,10 +29279,10 @@
         <v>127</v>
       </c>
       <c r="B184" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C184" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="12.75">
@@ -29290,10 +29290,10 @@
         <v>127</v>
       </c>
       <c r="B185" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C185" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="12.75">
@@ -29301,10 +29301,10 @@
         <v>127</v>
       </c>
       <c r="B186" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C186" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="12.75">
@@ -29312,10 +29312,10 @@
         <v>127</v>
       </c>
       <c r="B187" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C187" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="12.75">
@@ -29323,10 +29323,10 @@
         <v>127</v>
       </c>
       <c r="B188" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C188" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="12.75">
@@ -29334,10 +29334,10 @@
         <v>127</v>
       </c>
       <c r="B189" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C189" s="23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="12.75">
@@ -29345,10 +29345,10 @@
         <v>127</v>
       </c>
       <c r="B190" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C190" s="23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="12.75">
@@ -29356,10 +29356,10 @@
         <v>127</v>
       </c>
       <c r="B191" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C191" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="12.75">
@@ -29367,10 +29367,10 @@
         <v>127</v>
       </c>
       <c r="B192" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C192" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="12.75">
@@ -29378,10 +29378,10 @@
         <v>127</v>
       </c>
       <c r="B193" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C193" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="12.75">
@@ -29389,10 +29389,10 @@
         <v>127</v>
       </c>
       <c r="B194" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C194" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="12.75">
@@ -29400,10 +29400,10 @@
         <v>173</v>
       </c>
       <c r="B195" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C195" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="12.75">
@@ -29411,10 +29411,10 @@
         <v>173</v>
       </c>
       <c r="B196" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C196" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="12.75">
@@ -29422,10 +29422,10 @@
         <v>173</v>
       </c>
       <c r="B197" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C197" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="12.75">
@@ -29433,10 +29433,10 @@
         <v>173</v>
       </c>
       <c r="B198" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C198" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="12.75">
@@ -29444,10 +29444,10 @@
         <v>173</v>
       </c>
       <c r="B199" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C199" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="12.75">
@@ -29455,10 +29455,10 @@
         <v>173</v>
       </c>
       <c r="B200" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C200" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="12.75">
@@ -29466,10 +29466,10 @@
         <v>173</v>
       </c>
       <c r="B201" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C201" s="23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="12.75">
@@ -29477,10 +29477,10 @@
         <v>173</v>
       </c>
       <c r="B202" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C202" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="12.75">
@@ -29488,10 +29488,10 @@
         <v>173</v>
       </c>
       <c r="B203" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C203" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="12.75">
@@ -29499,10 +29499,10 @@
         <v>173</v>
       </c>
       <c r="B204" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C204" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="12.75">
@@ -29510,10 +29510,10 @@
         <v>173</v>
       </c>
       <c r="B205" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C205" s="23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="12.75">
@@ -29521,219 +29521,219 @@
         <v>173</v>
       </c>
       <c r="B206" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C206" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="12.75">
       <c r="A207" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B207" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C207" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="12.75">
       <c r="A208" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B208" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C208" s="23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="12.75">
       <c r="A209" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B209" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C209" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="12.75">
       <c r="A210" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B210" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C210" s="23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="12.75">
       <c r="A211" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B211" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C211" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="12.75">
       <c r="A212" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B212" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C212" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="12.75">
       <c r="A213" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B213" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C213" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="12.75">
       <c r="A214" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B214" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C214" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="12.75">
       <c r="A215" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B215" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C215" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="12.75">
       <c r="A216" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B216" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C216" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="12.75">
       <c r="A217" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B217" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C217" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="12.75">
       <c r="A218" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B218" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C218" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="12.75">
       <c r="A219" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B219" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C219" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="12.75">
       <c r="A220" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B220" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C220" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="12.75">
       <c r="A221" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B221" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C221" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="12.75">
       <c r="A222" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B222" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C222" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="12.75">
       <c r="A223" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B223" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C223" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="12.75">
       <c r="A224" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B224" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C224" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="12.75">
       <c r="A225" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B225" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C225" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="12.75">
@@ -29741,10 +29741,10 @@
         <v>144</v>
       </c>
       <c r="B226" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C226" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="12.75">
@@ -29752,10 +29752,10 @@
         <v>144</v>
       </c>
       <c r="B227" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C227" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="12.75">
@@ -29763,10 +29763,10 @@
         <v>144</v>
       </c>
       <c r="B228" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C228" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="12.75">
@@ -29774,10 +29774,10 @@
         <v>144</v>
       </c>
       <c r="B229" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C229" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="12.75">
@@ -29785,10 +29785,10 @@
         <v>144</v>
       </c>
       <c r="B230" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C230" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="12.75">
@@ -29796,10 +29796,10 @@
         <v>144</v>
       </c>
       <c r="B231" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C231" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="12.75">
@@ -29807,10 +29807,10 @@
         <v>144</v>
       </c>
       <c r="B232" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C232" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="12.75">
@@ -29818,10 +29818,10 @@
         <v>144</v>
       </c>
       <c r="B233" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C233" s="23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="12.75">
@@ -29829,10 +29829,10 @@
         <v>144</v>
       </c>
       <c r="B234" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C234" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="12.75">
@@ -29840,10 +29840,10 @@
         <v>144</v>
       </c>
       <c r="B235" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C235" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="12.75">
@@ -29851,10 +29851,10 @@
         <v>144</v>
       </c>
       <c r="B236" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C236" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="12.75">
@@ -29862,10 +29862,10 @@
         <v>144</v>
       </c>
       <c r="B237" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C237" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="12.75">
@@ -29873,10 +29873,10 @@
         <v>144</v>
       </c>
       <c r="B238" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C238" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="12.75">
@@ -29884,10 +29884,10 @@
         <v>144</v>
       </c>
       <c r="B239" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C239" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="12.75">
@@ -29895,10 +29895,10 @@
         <v>144</v>
       </c>
       <c r="B240" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C240" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="12.75">
@@ -29906,10 +29906,10 @@
         <v>144</v>
       </c>
       <c r="B241" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C241" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="12.75">
@@ -29917,10 +29917,10 @@
         <v>144</v>
       </c>
       <c r="B242" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C242" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="12.75">
@@ -29928,10 +29928,10 @@
         <v>144</v>
       </c>
       <c r="B243" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C243" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="12.75">
@@ -29939,10 +29939,10 @@
         <v>144</v>
       </c>
       <c r="B244" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C244" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>